<commit_message>
Updated global unit test for BC Workspace
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/BC_FGP_XML_BUILDER_PROD_04/met/XLSX_etalon_1/xlsx_etalon_1.xlsx
+++ b/FME_files/UNIT_TESTS/BC_FGP_XML_BUILDER_PROD_04/met/XLSX_etalon_1/xlsx_etalon_1.xlsx
@@ -6,16 +6,32 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="SPATIAL_TYPE_NOT_MAPPED" sheetId="1" r:id="rId2"/>
+    <sheet name="GEOSPATIAL_FORMAT_NOT_MAPPED" sheetId="1" r:id="rId2"/>
+    <sheet name="SPATIAL_TYPE_NOT_MAPPED" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>_timestamp</t>
+  </si>
+  <si>
+    <t>30aeb5c1-4285-46c8-b60b-15b1a6f4258b</t>
+  </si>
+  <si>
+    <t>fgdb</t>
+  </si>
+  <si>
+    <t>20201112</t>
   </si>
   <si>
     <t>notes</t>
@@ -24,28 +40,10 @@
     <t>title</t>
   </si>
   <si>
-    <t>_timestamp</t>
-  </si>
-  <si>
-    <t>30aeb5c1-4285-46c8-b60b-15b1a6f4258b</t>
-  </si>
-  <si>
     <t>This dataset consists of polyline, single part, and multi part polygons representing the Province of British Columbia. The terrestrial portion of the boundary was derived from the [Province of British Columbia - Legally Defined Administrative Areas of BC: WHSE_LEGAL_ADMIN_BOUNDARIES.ABMS_PROVINCE_SP](https://catalogue.data.gov.bc.ca/dataset/a7e32e45-63ae-4f5a-9275-9402b6deebdc). The coastal portion of the boundary differs from the ABMS boundary and was derived from the [Freshwater Atlas Coastlines: WHSE_BASEMAPPING.FWA_COASTLINES_SP](https://catalogue.data.gov.bc.ca/dataset/87b1d6a7-d4d1-4c25-a879-233becdbffed). This boundary may be updated periodically, as more accurate data becomes available. Due to the structure of the data, it does not meet the technical requirements to be published in the BC Geographic Warehouse (BCGW). It is available for download as a file geodatabase in the Data and Resources section below.</t>
   </si>
   <si>
     <t>Province of British Columbia - Boundary Terrestrial</t>
-  </si>
-  <si>
-    <t>20200911</t>
-  </si>
-  <si>
-    <t>5b75978f-02b9-457b-9dd4-71f0927bf7dc</t>
-  </si>
-  <si>
-    <t>Terrestrial Ecosystem Mapping for Fort Sheppard in the Arrow Boundary Forest District (ttem_fs)</t>
-  </si>
-  <si>
-    <t>Terrestrial Ecosystem Mapping - Fort Sheppard</t>
   </si>
 </sst>
 </file>
@@ -94,7 +92,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="true"/>
+    <col min="2" max="2" width="8.7109375" customWidth="true"/>
+    <col min="3" max="3" width="20.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="true"/>
@@ -108,41 +142,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>